<commit_message>
Mô tả ngắn về thay đổi của bạn
</commit_message>
<xml_diff>
--- a/Stock_data/Alphabet.xlsx
+++ b/Stock_data/Alphabet.xlsx
@@ -778,7 +778,7 @@
         <v>43847</v>
       </c>
       <c r="B15" t="n">
-        <v>73.83816528320312</v>
+        <v>73.83817291259766</v>
       </c>
       <c r="C15" t="n">
         <v>74.01950073242188</v>
@@ -916,7 +916,7 @@
         <v>43858</v>
       </c>
       <c r="B21" t="n">
-        <v>72.45008087158203</v>
+        <v>72.4500732421875</v>
       </c>
       <c r="C21" t="n">
         <v>72.62799835205078</v>
@@ -939,7 +939,7 @@
         <v>43859</v>
       </c>
       <c r="B22" t="n">
-        <v>72.75283050537109</v>
+        <v>72.75283813476562</v>
       </c>
       <c r="C22" t="n">
         <v>72.93150329589844</v>
@@ -1031,7 +1031,7 @@
         <v>43865</v>
       </c>
       <c r="B26" t="n">
-        <v>72.17624664306641</v>
+        <v>72.17625427246094</v>
       </c>
       <c r="C26" t="n">
         <v>72.35350036621094</v>
@@ -1123,7 +1123,7 @@
         <v>43871</v>
       </c>
       <c r="B30" t="n">
-        <v>75.24920654296875</v>
+        <v>75.24919891357422</v>
       </c>
       <c r="C30" t="n">
         <v>75.43399810791016</v>
@@ -1146,7 +1146,7 @@
         <v>43872</v>
       </c>
       <c r="B31" t="n">
-        <v>75.25469207763672</v>
+        <v>75.25468444824219</v>
       </c>
       <c r="C31" t="n">
         <v>75.43949890136719</v>
@@ -1307,7 +1307,7 @@
         <v>43882</v>
       </c>
       <c r="B38" t="n">
-        <v>74.07358551025391</v>
+        <v>74.07359313964844</v>
       </c>
       <c r="C38" t="n">
         <v>74.25550079345703</v>
@@ -1353,7 +1353,7 @@
         <v>43886</v>
       </c>
       <c r="B40" t="n">
-        <v>69.25242614746094</v>
+        <v>69.25243377685547</v>
       </c>
       <c r="C40" t="n">
         <v>69.42250061035156</v>
@@ -1491,7 +1491,7 @@
         <v>43894</v>
       </c>
       <c r="B46" t="n">
-        <v>69.15616607666016</v>
+        <v>69.15615844726562</v>
       </c>
       <c r="C46" t="n">
         <v>69.32599639892578</v>
@@ -1629,7 +1629,7 @@
         <v>43902</v>
       </c>
       <c r="B52" t="n">
-        <v>55.60893630981445</v>
+        <v>55.60893249511719</v>
       </c>
       <c r="C52" t="n">
         <v>55.74549865722656</v>
@@ -1652,7 +1652,7 @@
         <v>43903</v>
       </c>
       <c r="B53" t="n">
-        <v>60.83709335327148</v>
+        <v>60.83709716796875</v>
       </c>
       <c r="C53" t="n">
         <v>60.98649978637695</v>
@@ -1721,7 +1721,7 @@
         <v>43908</v>
       </c>
       <c r="B56" t="n">
-        <v>54.70565032958984</v>
+        <v>54.70565414428711</v>
       </c>
       <c r="C56" t="n">
         <v>54.84000015258789</v>
@@ -1813,7 +1813,7 @@
         <v>43914</v>
       </c>
       <c r="B60" t="n">
-        <v>56.58403778076172</v>
+        <v>56.58404159545898</v>
       </c>
       <c r="C60" t="n">
         <v>56.72299957275391</v>
@@ -1905,7 +1905,7 @@
         <v>43920</v>
       </c>
       <c r="B64" t="n">
-        <v>57.20052337646484</v>
+        <v>57.20052719116211</v>
       </c>
       <c r="C64" t="n">
         <v>57.34099960327148</v>
@@ -1951,7 +1951,7 @@
         <v>43922</v>
       </c>
       <c r="B66" t="n">
-        <v>55.14556884765625</v>
+        <v>55.14557266235352</v>
       </c>
       <c r="C66" t="n">
         <v>55.28099822998047</v>
@@ -1974,7 +1974,7 @@
         <v>43923</v>
       </c>
       <c r="B67" t="n">
-        <v>55.90470504760742</v>
+        <v>55.90470886230469</v>
       </c>
       <c r="C67" t="n">
         <v>56.04199981689453</v>
@@ -2066,7 +2066,7 @@
         <v>43929</v>
       </c>
       <c r="B71" t="n">
-        <v>60.36575317382812</v>
+        <v>60.36574935913086</v>
       </c>
       <c r="C71" t="n">
         <v>60.51399993896484</v>
@@ -2135,7 +2135,7 @@
         <v>43935</v>
       </c>
       <c r="B74" t="n">
-        <v>63.30602645874023</v>
+        <v>63.3060302734375</v>
       </c>
       <c r="C74" t="n">
         <v>63.46149826049805</v>
@@ -2204,7 +2204,7 @@
         <v>43938</v>
       </c>
       <c r="B77" t="n">
-        <v>64.00531768798828</v>
+        <v>64.00531005859375</v>
       </c>
       <c r="C77" t="n">
         <v>64.16249847412109</v>
@@ -2411,7 +2411,7 @@
         <v>43951</v>
       </c>
       <c r="B86" t="n">
-        <v>67.26780700683594</v>
+        <v>67.26779937744141</v>
       </c>
       <c r="C86" t="n">
         <v>67.43299865722656</v>
@@ -2549,7 +2549,7 @@
         <v>43959</v>
       </c>
       <c r="B92" t="n">
-        <v>69.24844360351562</v>
+        <v>69.24843597412109</v>
       </c>
       <c r="C92" t="n">
         <v>69.41850280761719</v>
@@ -2595,7 +2595,7 @@
         <v>43963</v>
       </c>
       <c r="B94" t="n">
-        <v>68.61849212646484</v>
+        <v>68.61848449707031</v>
       </c>
       <c r="C94" t="n">
         <v>68.78700256347656</v>
@@ -2664,7 +2664,7 @@
         <v>43966</v>
       </c>
       <c r="B97" t="n">
-        <v>68.49130249023438</v>
+        <v>68.49129486083984</v>
       </c>
       <c r="C97" t="n">
         <v>68.65950012207031</v>
@@ -2687,7 +2687,7 @@
         <v>43969</v>
       </c>
       <c r="B98" t="n">
-        <v>69.02748107910156</v>
+        <v>69.02747344970703</v>
       </c>
       <c r="C98" t="n">
         <v>69.19699859619141</v>
@@ -3032,7 +3032,7 @@
         <v>43991</v>
       </c>
       <c r="B113" t="n">
-        <v>72.629638671875</v>
+        <v>72.62963104248047</v>
       </c>
       <c r="C113" t="n">
         <v>72.80799865722656</v>
@@ -3101,7 +3101,7 @@
         <v>43994</v>
       </c>
       <c r="B116" t="n">
-        <v>70.48589324951172</v>
+        <v>70.48590087890625</v>
       </c>
       <c r="C116" t="n">
         <v>70.65899658203125</v>
@@ -3170,7 +3170,7 @@
         <v>43999</v>
       </c>
       <c r="B119" t="n">
-        <v>72.37825012207031</v>
+        <v>72.37825775146484</v>
       </c>
       <c r="C119" t="n">
         <v>72.55599975585938</v>
@@ -3239,7 +3239,7 @@
         <v>44004</v>
       </c>
       <c r="B122" t="n">
-        <v>72.41516876220703</v>
+        <v>72.4151611328125</v>
       </c>
       <c r="C122" t="n">
         <v>72.59300231933594</v>
@@ -3354,7 +3354,7 @@
         <v>44011</v>
       </c>
       <c r="B127" t="n">
-        <v>69.57762908935547</v>
+        <v>69.57762145996094</v>
       </c>
       <c r="C127" t="n">
         <v>69.74849700927734</v>
@@ -3446,7 +3446,7 @@
         <v>44018</v>
       </c>
       <c r="B131" t="n">
-        <v>74.60179138183594</v>
+        <v>74.60179901123047</v>
       </c>
       <c r="C131" t="n">
         <v>74.78500366210938</v>
@@ -3469,7 +3469,7 @@
         <v>44019</v>
       </c>
       <c r="B132" t="n">
-        <v>74.07708740234375</v>
+        <v>74.07707977294922</v>
       </c>
       <c r="C132" t="n">
         <v>74.25900268554688</v>
@@ -3561,7 +3561,7 @@
         <v>44025</v>
       </c>
       <c r="B136" t="n">
-        <v>75.38188171386719</v>
+        <v>75.38187408447266</v>
       </c>
       <c r="C136" t="n">
         <v>75.56700134277344</v>
@@ -3607,7 +3607,7 @@
         <v>44027</v>
       </c>
       <c r="B138" t="n">
-        <v>75.49659729003906</v>
+        <v>75.49658966064453</v>
       </c>
       <c r="C138" t="n">
         <v>75.68199920654297</v>
@@ -3653,7 +3653,7 @@
         <v>44029</v>
       </c>
       <c r="B140" t="n">
-        <v>75.59185028076172</v>
+        <v>75.59185791015625</v>
       </c>
       <c r="C140" t="n">
         <v>75.77749633789062</v>
@@ -3676,7 +3676,7 @@
         <v>44032</v>
       </c>
       <c r="B141" t="n">
-        <v>78.09422302246094</v>
+        <v>78.09421539306641</v>
       </c>
       <c r="C141" t="n">
         <v>78.28600311279297</v>
@@ -3722,7 +3722,7 @@
         <v>44034</v>
       </c>
       <c r="B143" t="n">
-        <v>78.23237609863281</v>
+        <v>78.23236846923828</v>
       </c>
       <c r="C143" t="n">
         <v>78.42449951171875</v>
@@ -3906,7 +3906,7 @@
         <v>44046</v>
       </c>
       <c r="B151" t="n">
-        <v>73.54189300537109</v>
+        <v>73.54190063476562</v>
       </c>
       <c r="C151" t="n">
         <v>73.72250366210938</v>
@@ -3929,7 +3929,7 @@
         <v>44047</v>
       </c>
       <c r="B152" t="n">
-        <v>73.06905364990234</v>
+        <v>73.06904602050781</v>
       </c>
       <c r="C152" t="n">
         <v>73.24849700927734</v>
@@ -3975,7 +3975,7 @@
         <v>44049</v>
       </c>
       <c r="B154" t="n">
-        <v>74.82124328613281</v>
+        <v>74.82125091552734</v>
       </c>
       <c r="C154" t="n">
         <v>75.00499725341797</v>
@@ -4044,7 +4044,7 @@
         <v>44054</v>
       </c>
       <c r="B157" t="n">
-        <v>73.83467864990234</v>
+        <v>73.83467102050781</v>
       </c>
       <c r="C157" t="n">
         <v>74.01599884033203</v>
@@ -4067,7 +4067,7 @@
         <v>44055</v>
       </c>
       <c r="B158" t="n">
-        <v>75.14645385742188</v>
+        <v>75.14646148681641</v>
       </c>
       <c r="C158" t="n">
         <v>75.33100128173828</v>
@@ -4090,7 +4090,7 @@
         <v>44056</v>
       </c>
       <c r="B159" t="n">
-        <v>75.73650360107422</v>
+        <v>75.73651123046875</v>
       </c>
       <c r="C159" t="n">
         <v>75.92250061035156</v>
@@ -4113,7 +4113,7 @@
         <v>44057</v>
       </c>
       <c r="B160" t="n">
-        <v>75.20182037353516</v>
+        <v>75.20181274414062</v>
       </c>
       <c r="C160" t="n">
         <v>75.38649749755859</v>
@@ -4228,7 +4228,7 @@
         <v>44064</v>
       </c>
       <c r="B165" t="n">
-        <v>78.82741546630859</v>
+        <v>78.82742309570312</v>
       </c>
       <c r="C165" t="n">
         <v>79.02100372314453</v>
@@ -4251,7 +4251,7 @@
         <v>44067</v>
       </c>
       <c r="B166" t="n">
-        <v>79.21546173095703</v>
+        <v>79.21546936035156</v>
       </c>
       <c r="C166" t="n">
         <v>79.41000366210938</v>
@@ -4343,7 +4343,7 @@
         <v>44071</v>
       </c>
       <c r="B170" t="n">
-        <v>82.01906585693359</v>
+        <v>82.01907348632812</v>
       </c>
       <c r="C170" t="n">
         <v>82.22049713134766</v>
@@ -4573,7 +4573,7 @@
         <v>44088</v>
       </c>
       <c r="B180" t="n">
-        <v>75.77790069580078</v>
+        <v>75.77789306640625</v>
       </c>
       <c r="C180" t="n">
         <v>75.96399688720703</v>
@@ -4596,7 +4596,7 @@
         <v>44089</v>
       </c>
       <c r="B181" t="n">
-        <v>76.88318634033203</v>
+        <v>76.88319396972656</v>
       </c>
       <c r="C181" t="n">
         <v>77.07199859619141</v>
@@ -4711,7 +4711,7 @@
         <v>44096</v>
       </c>
       <c r="B186" t="n">
-        <v>73.09349060058594</v>
+        <v>73.09349822998047</v>
       </c>
       <c r="C186" t="n">
         <v>73.27300262451172</v>
@@ -4849,7 +4849,7 @@
         <v>44104</v>
       </c>
       <c r="B192" t="n">
-        <v>73.29999542236328</v>
+        <v>73.29998779296875</v>
       </c>
       <c r="C192" t="n">
         <v>73.48000335693359</v>
@@ -4987,7 +4987,7 @@
         <v>44112</v>
       </c>
       <c r="B198" t="n">
-        <v>74.11448669433594</v>
+        <v>74.11449432373047</v>
       </c>
       <c r="C198" t="n">
         <v>74.29650115966797</v>
@@ -5056,7 +5056,7 @@
         <v>44117</v>
       </c>
       <c r="B201" t="n">
-        <v>78.3914794921875</v>
+        <v>78.39148712158203</v>
       </c>
       <c r="C201" t="n">
         <v>78.58399963378906</v>
@@ -5125,7 +5125,7 @@
         <v>44120</v>
       </c>
       <c r="B204" t="n">
-        <v>78.45781707763672</v>
+        <v>78.45782470703125</v>
       </c>
       <c r="C204" t="n">
         <v>78.65049743652344</v>
@@ -5194,7 +5194,7 @@
         <v>44125</v>
       </c>
       <c r="B207" t="n">
-        <v>79.47032928466797</v>
+        <v>79.4703369140625</v>
       </c>
       <c r="C207" t="n">
         <v>79.66549682617188</v>
@@ -5286,7 +5286,7 @@
         <v>44131</v>
       </c>
       <c r="B211" t="n">
-        <v>80.01649475097656</v>
+        <v>80.01648712158203</v>
       </c>
       <c r="C211" t="n">
         <v>80.21299743652344</v>
@@ -5401,7 +5401,7 @@
         <v>44138</v>
       </c>
       <c r="B216" t="n">
-        <v>82.30836486816406</v>
+        <v>82.30835723876953</v>
       </c>
       <c r="C216" t="n">
         <v>82.510498046875</v>
@@ -5654,7 +5654,7 @@
         <v>44153</v>
       </c>
       <c r="B227" t="n">
-        <v>87.12503814697266</v>
+        <v>87.12503051757812</v>
       </c>
       <c r="C227" t="n">
         <v>87.33899688720703</v>
@@ -5746,7 +5746,7 @@
         <v>44159</v>
       </c>
       <c r="B231" t="n">
-        <v>88.22732543945312</v>
+        <v>88.22733306884766</v>
       </c>
       <c r="C231" t="n">
         <v>88.44400024414062</v>
@@ -5769,7 +5769,7 @@
         <v>44160</v>
       </c>
       <c r="B232" t="n">
-        <v>88.35451507568359</v>
+        <v>88.35452270507812</v>
       </c>
       <c r="C232" t="n">
         <v>88.57150268554688</v>
@@ -5792,7 +5792,7 @@
         <v>44162</v>
       </c>
       <c r="B233" t="n">
-        <v>89.43984985351562</v>
+        <v>89.43985748291016</v>
       </c>
       <c r="C233" t="n">
         <v>89.65950012207031</v>
@@ -5838,7 +5838,7 @@
         <v>44166</v>
       </c>
       <c r="B235" t="n">
-        <v>89.68475341796875</v>
+        <v>89.68474578857422</v>
       </c>
       <c r="C235" t="n">
         <v>89.90499877929688</v>
@@ -6022,7 +6022,7 @@
         <v>44176</v>
       </c>
       <c r="B243" t="n">
-        <v>88.87024688720703</v>
+        <v>88.87025451660156</v>
       </c>
       <c r="C243" t="n">
         <v>89.0885009765625</v>
@@ -6068,7 +6068,7 @@
         <v>44180</v>
       </c>
       <c r="B245" t="n">
-        <v>88.17195892333984</v>
+        <v>88.17196655273438</v>
       </c>
       <c r="C245" t="n">
         <v>88.38849639892578</v>
@@ -6321,7 +6321,7 @@
         <v>44196</v>
       </c>
       <c r="B256" t="n">
-        <v>87.37941741943359</v>
+        <v>87.37940979003906</v>
       </c>
       <c r="C256" t="n">
         <v>87.59400177001953</v>
@@ -6413,7 +6413,7 @@
         <v>44203</v>
       </c>
       <c r="B260" t="n">
-        <v>89.14357757568359</v>
+        <v>89.14358520507812</v>
       </c>
       <c r="C260" t="n">
         <v>89.36250305175781</v>
@@ -6459,7 +6459,7 @@
         <v>44207</v>
       </c>
       <c r="B262" t="n">
-        <v>88.11959075927734</v>
+        <v>88.11959838867188</v>
       </c>
       <c r="C262" t="n">
         <v>88.33599853515625</v>
@@ -6574,7 +6574,7 @@
         <v>44215</v>
       </c>
       <c r="B267" t="n">
-        <v>89.32363128662109</v>
+        <v>89.32363891601562</v>
       </c>
       <c r="C267" t="n">
         <v>89.54299926757812</v>
@@ -6643,7 +6643,7 @@
         <v>44218</v>
       </c>
       <c r="B270" t="n">
-        <v>94.81964111328125</v>
+        <v>94.81963348388672</v>
       </c>
       <c r="C270" t="n">
         <v>95.05249786376953</v>
@@ -6735,7 +6735,7 @@
         <v>44224</v>
       </c>
       <c r="B274" t="n">
-        <v>92.92728424072266</v>
+        <v>92.92729187011719</v>
       </c>
       <c r="C274" t="n">
         <v>93.15550231933594</v>
@@ -6781,7 +6781,7 @@
         <v>44228</v>
       </c>
       <c r="B276" t="n">
-        <v>94.8345947265625</v>
+        <v>94.83460235595703</v>
       </c>
       <c r="C276" t="n">
         <v>95.06749725341797</v>
@@ -6804,7 +6804,7 @@
         <v>44229</v>
       </c>
       <c r="B277" t="n">
-        <v>96.139404296875</v>
+        <v>96.13939666748047</v>
       </c>
       <c r="C277" t="n">
         <v>96.37550354003906</v>
@@ -6850,7 +6850,7 @@
         <v>44231</v>
       </c>
       <c r="B279" t="n">
-        <v>102.8658828735352</v>
+        <v>102.8658752441406</v>
       </c>
       <c r="C279" t="n">
         <v>103.1184997558594</v>
@@ -6873,7 +6873,7 @@
         <v>44232</v>
       </c>
       <c r="B280" t="n">
-        <v>104.6430206298828</v>
+        <v>104.6430130004883</v>
       </c>
       <c r="C280" t="n">
         <v>104.9000015258789</v>
@@ -6965,7 +6965,7 @@
         <v>44238</v>
       </c>
       <c r="B284" t="n">
-        <v>104.5377731323242</v>
+        <v>104.5377807617188</v>
       </c>
       <c r="C284" t="n">
         <v>104.7945022583008</v>
@@ -6988,7 +6988,7 @@
         <v>44239</v>
       </c>
       <c r="B285" t="n">
-        <v>104.9477615356445</v>
+        <v>104.9477691650391</v>
       </c>
       <c r="C285" t="n">
         <v>105.2054977416992</v>
@@ -7057,7 +7057,7 @@
         <v>44245</v>
       </c>
       <c r="B288" t="n">
-        <v>105.6006698608398</v>
+        <v>105.6006622314453</v>
       </c>
       <c r="C288" t="n">
         <v>105.8600006103516</v>
@@ -7126,7 +7126,7 @@
         <v>44250</v>
       </c>
       <c r="B291" t="n">
-        <v>103.2893447875977</v>
+        <v>103.2893371582031</v>
       </c>
       <c r="C291" t="n">
         <v>103.5429992675781</v>
@@ -7172,7 +7172,7 @@
         <v>44252</v>
       </c>
       <c r="B293" t="n">
-        <v>101.3191757202148</v>
+        <v>101.3191833496094</v>
       </c>
       <c r="C293" t="n">
         <v>101.568000793457</v>
@@ -7241,7 +7241,7 @@
         <v>44257</v>
       </c>
       <c r="B296" t="n">
-        <v>103.5377349853516</v>
+        <v>103.537727355957</v>
       </c>
       <c r="C296" t="n">
         <v>103.7919998168945</v>
@@ -7310,7 +7310,7 @@
         <v>44260</v>
       </c>
       <c r="B299" t="n">
-        <v>105.1687240600586</v>
+        <v>105.1687316894531</v>
       </c>
       <c r="C299" t="n">
         <v>105.427001953125</v>
@@ -7402,7 +7402,7 @@
         <v>44266</v>
       </c>
       <c r="B303" t="n">
-        <v>105.4794692993164</v>
+        <v>105.4794616699219</v>
       </c>
       <c r="C303" t="n">
         <v>105.7385025024414</v>
@@ -7448,7 +7448,7 @@
         <v>44270</v>
       </c>
       <c r="B305" t="n">
-        <v>103.0713729858398</v>
+        <v>103.0713806152344</v>
       </c>
       <c r="C305" t="n">
         <v>103.3245010375977</v>
@@ -7471,7 +7471,7 @@
         <v>44271</v>
       </c>
       <c r="B306" t="n">
-        <v>104.3696823120117</v>
+        <v>104.3696899414062</v>
       </c>
       <c r="C306" t="n">
         <v>104.6259994506836</v>
@@ -7586,7 +7586,7 @@
         <v>44278</v>
       </c>
       <c r="B311" t="n">
-        <v>102.3965377807617</v>
+        <v>102.3965301513672</v>
       </c>
       <c r="C311" t="n">
         <v>102.6480026245117</v>
@@ -8000,7 +8000,7 @@
         <v>44305</v>
       </c>
       <c r="B329" t="n">
-        <v>114.8379821777344</v>
+        <v>114.8379745483398</v>
       </c>
       <c r="C329" t="n">
         <v>115.120002746582</v>
@@ -8023,7 +8023,7 @@
         <v>44306</v>
       </c>
       <c r="B330" t="n">
-        <v>114.4005508422852</v>
+        <v>114.4005584716797</v>
       </c>
       <c r="C330" t="n">
         <v>114.6815032958984</v>
@@ -8069,7 +8069,7 @@
         <v>44308</v>
       </c>
       <c r="B332" t="n">
-        <v>113.1182098388672</v>
+        <v>113.1182022094727</v>
       </c>
       <c r="C332" t="n">
         <v>113.3960037231445</v>
@@ -8092,7 +8092,7 @@
         <v>44309</v>
       </c>
       <c r="B333" t="n">
-        <v>115.4813995361328</v>
+        <v>115.4813919067383</v>
       </c>
       <c r="C333" t="n">
         <v>115.7649993896484</v>
@@ -8230,7 +8230,7 @@
         <v>44319</v>
       </c>
       <c r="B339" t="n">
-        <v>119.4651184082031</v>
+        <v>119.4651107788086</v>
       </c>
       <c r="C339" t="n">
         <v>119.7584991455078</v>
@@ -8299,7 +8299,7 @@
         <v>44322</v>
       </c>
       <c r="B342" t="n">
-        <v>118.7758102416992</v>
+        <v>118.7758026123047</v>
       </c>
       <c r="C342" t="n">
         <v>119.067497253418</v>
@@ -8460,7 +8460,7 @@
         <v>44333</v>
       </c>
       <c r="B349" t="n">
-        <v>115.7861480712891</v>
+        <v>115.7861557006836</v>
       </c>
       <c r="C349" t="n">
         <v>116.0705032348633</v>
@@ -8483,7 +8483,7 @@
         <v>44334</v>
       </c>
       <c r="B350" t="n">
-        <v>114.8893508911133</v>
+        <v>114.8893585205078</v>
       </c>
       <c r="C350" t="n">
         <v>115.171501159668</v>
@@ -8621,7 +8621,7 @@
         <v>44342</v>
       </c>
       <c r="B356" t="n">
-        <v>121.3784103393555</v>
+        <v>121.37841796875</v>
       </c>
       <c r="C356" t="n">
         <v>121.6764984130859</v>
@@ -8644,7 +8644,7 @@
         <v>44343</v>
       </c>
       <c r="B357" t="n">
-        <v>119.8312149047852</v>
+        <v>119.8312225341797</v>
       </c>
       <c r="C357" t="n">
         <v>120.1255035400391</v>
@@ -8667,7 +8667,7 @@
         <v>44344</v>
       </c>
       <c r="B358" t="n">
-        <v>120.2826156616211</v>
+        <v>120.2826080322266</v>
       </c>
       <c r="C358" t="n">
         <v>120.5780029296875</v>
@@ -8690,7 +8690,7 @@
         <v>44348</v>
       </c>
       <c r="B359" t="n">
-        <v>121.19287109375</v>
+        <v>121.1928787231445</v>
       </c>
       <c r="C359" t="n">
         <v>121.4905014038086</v>
@@ -8897,7 +8897,7 @@
         <v>44361</v>
       </c>
       <c r="B368" t="n">
-        <v>126.0424652099609</v>
+        <v>126.0424575805664</v>
       </c>
       <c r="C368" t="n">
         <v>126.3519973754883</v>
@@ -9173,7 +9173,7 @@
         <v>44377</v>
       </c>
       <c r="B380" t="n">
-        <v>125.0090026855469</v>
+        <v>125.0089950561523</v>
       </c>
       <c r="C380" t="n">
         <v>125.3160018920898</v>
@@ -9288,7 +9288,7 @@
         <v>44385</v>
       </c>
       <c r="B385" t="n">
-        <v>128.8605346679688</v>
+        <v>128.8605499267578</v>
       </c>
       <c r="C385" t="n">
         <v>129.177001953125</v>
@@ -9311,7 +9311,7 @@
         <v>44386</v>
       </c>
       <c r="B386" t="n">
-        <v>129.2570648193359</v>
+        <v>129.2570495605469</v>
       </c>
       <c r="C386" t="n">
         <v>129.5744934082031</v>
@@ -9403,7 +9403,7 @@
         <v>44392</v>
       </c>
       <c r="B390" t="n">
-        <v>130.9449157714844</v>
+        <v>130.9449310302734</v>
       </c>
       <c r="C390" t="n">
         <v>131.2664947509766</v>
@@ -9426,7 +9426,7 @@
         <v>44393</v>
       </c>
       <c r="B391" t="n">
-        <v>131.5225219726562</v>
+        <v>131.5225067138672</v>
       </c>
       <c r="C391" t="n">
         <v>131.8455047607422</v>
@@ -9449,7 +9449,7 @@
         <v>44396</v>
       </c>
       <c r="B392" t="n">
-        <v>128.9373626708984</v>
+        <v>128.9373474121094</v>
       </c>
       <c r="C392" t="n">
         <v>129.2539978027344</v>
@@ -9541,7 +9541,7 @@
         <v>44400</v>
       </c>
       <c r="B396" t="n">
-        <v>137.4783782958984</v>
+        <v>137.4783630371094</v>
       </c>
       <c r="C396" t="n">
         <v>137.8159942626953</v>
@@ -9587,7 +9587,7 @@
         <v>44404</v>
       </c>
       <c r="B398" t="n">
-        <v>136.4613800048828</v>
+        <v>136.4613647460938</v>
       </c>
       <c r="C398" t="n">
         <v>136.7964935302734</v>
@@ -9633,7 +9633,7 @@
         <v>44406</v>
       </c>
       <c r="B400" t="n">
-        <v>136.2060089111328</v>
+        <v>136.2059936523438</v>
       </c>
       <c r="C400" t="n">
         <v>136.5404968261719</v>
@@ -9702,7 +9702,7 @@
         <v>44411</v>
       </c>
       <c r="B403" t="n">
-        <v>135.9461364746094</v>
+        <v>135.9461517333984</v>
       </c>
       <c r="C403" t="n">
         <v>136.2799987792969</v>
@@ -9725,7 +9725,7 @@
         <v>44412</v>
       </c>
       <c r="B404" t="n">
-        <v>135.6952667236328</v>
+        <v>135.6952514648438</v>
       </c>
       <c r="C404" t="n">
         <v>136.0285034179688</v>
@@ -9771,7 +9771,7 @@
         <v>44414</v>
       </c>
       <c r="B406" t="n">
-        <v>136.7002868652344</v>
+        <v>136.7002716064453</v>
       </c>
       <c r="C406" t="n">
         <v>137.0359954833984</v>
@@ -9794,7 +9794,7 @@
         <v>44417</v>
       </c>
       <c r="B407" t="n">
-        <v>137.6639251708984</v>
+        <v>137.6639099121094</v>
       </c>
       <c r="C407" t="n">
         <v>138.0019989013672</v>
@@ -9817,7 +9817,7 @@
         <v>44418</v>
       </c>
       <c r="B408" t="n">
-        <v>137.7581939697266</v>
+        <v>137.7581787109375</v>
       </c>
       <c r="C408" t="n">
         <v>138.0964965820312</v>
@@ -9863,7 +9863,7 @@
         <v>44420</v>
       </c>
       <c r="B410" t="n">
-        <v>138.0504608154297</v>
+        <v>138.0504760742188</v>
       </c>
       <c r="C410" t="n">
         <v>138.3894958496094</v>
@@ -9886,7 +9886,7 @@
         <v>44421</v>
       </c>
       <c r="B411" t="n">
-        <v>138.0669403076172</v>
+        <v>138.0669250488281</v>
       </c>
       <c r="C411" t="n">
         <v>138.406005859375</v>
@@ -9932,7 +9932,7 @@
         <v>44425</v>
       </c>
       <c r="B413" t="n">
-        <v>136.9641418457031</v>
+        <v>136.9641571044922</v>
       </c>
       <c r="C413" t="n">
         <v>137.3005065917969</v>
@@ -10231,7 +10231,7 @@
         <v>44442</v>
       </c>
       <c r="B426" t="n">
-        <v>144.4203186035156</v>
+        <v>144.4203338623047</v>
       </c>
       <c r="C426" t="n">
         <v>144.7749938964844</v>
@@ -10392,7 +10392,7 @@
         <v>44454</v>
       </c>
       <c r="B433" t="n">
-        <v>144.8502655029297</v>
+        <v>144.8502807617188</v>
       </c>
       <c r="C433" t="n">
         <v>145.2059936523438</v>
@@ -10461,7 +10461,7 @@
         <v>44459</v>
       </c>
       <c r="B436" t="n">
-        <v>138.6764221191406</v>
+        <v>138.6764373779297</v>
       </c>
       <c r="C436" t="n">
         <v>139.0169982910156</v>
@@ -10484,7 +10484,7 @@
         <v>44460</v>
       </c>
       <c r="B437" t="n">
-        <v>139.3043823242188</v>
+        <v>139.3043975830078</v>
       </c>
       <c r="C437" t="n">
         <v>139.6464996337891</v>
@@ -10599,7 +10599,7 @@
         <v>44467</v>
       </c>
       <c r="B442" t="n">
-        <v>135.8503723144531</v>
+        <v>135.8503875732422</v>
       </c>
       <c r="C442" t="n">
         <v>136.1840057373047</v>
@@ -10760,7 +10760,7 @@
         <v>44476</v>
       </c>
       <c r="B449" t="n">
-        <v>138.8445281982422</v>
+        <v>138.8445129394531</v>
       </c>
       <c r="C449" t="n">
         <v>139.1855010986328</v>
@@ -10829,7 +10829,7 @@
         <v>44481</v>
       </c>
       <c r="B452" t="n">
-        <v>136.3780822753906</v>
+        <v>136.3780670166016</v>
       </c>
       <c r="C452" t="n">
         <v>136.7129974365234</v>
@@ -10852,7 +10852,7 @@
         <v>44482</v>
       </c>
       <c r="B453" t="n">
-        <v>137.5621795654297</v>
+        <v>137.5621643066406</v>
       </c>
       <c r="C453" t="n">
         <v>137.8999938964844</v>
@@ -11036,7 +11036,7 @@
         <v>44494</v>
       </c>
       <c r="B461" t="n">
-        <v>138.4330139160156</v>
+        <v>138.4330291748047</v>
       </c>
       <c r="C461" t="n">
         <v>138.7729949951172</v>
@@ -11059,7 +11059,7 @@
         <v>44495</v>
       </c>
       <c r="B462" t="n">
-        <v>139.329833984375</v>
+        <v>139.3298187255859</v>
       </c>
       <c r="C462" t="n">
         <v>139.6719970703125</v>
@@ -11128,7 +11128,7 @@
         <v>44498</v>
       </c>
       <c r="B465" t="n">
-        <v>147.9072570800781</v>
+        <v>147.9072723388672</v>
       </c>
       <c r="C465" t="n">
         <v>148.2704925537109</v>
@@ -11174,7 +11174,7 @@
         <v>44502</v>
       </c>
       <c r="B467" t="n">
-        <v>145.5056610107422</v>
+        <v>145.5056762695312</v>
       </c>
       <c r="C467" t="n">
         <v>145.8630065917969</v>
@@ -11243,7 +11243,7 @@
         <v>44505</v>
       </c>
       <c r="B470" t="n">
-        <v>148.8753967285156</v>
+        <v>148.8753814697266</v>
       </c>
       <c r="C470" t="n">
         <v>149.2409973144531</v>
@@ -11312,7 +11312,7 @@
         <v>44510</v>
       </c>
       <c r="B473" t="n">
-        <v>146.2668151855469</v>
+        <v>146.2667999267578</v>
       </c>
       <c r="C473" t="n">
         <v>146.6260070800781</v>
@@ -11335,7 +11335,7 @@
         <v>44511</v>
       </c>
       <c r="B474" t="n">
-        <v>146.3884887695312</v>
+        <v>146.3885040283203</v>
       </c>
       <c r="C474" t="n">
         <v>146.7480010986328</v>
@@ -11358,7 +11358,7 @@
         <v>44512</v>
       </c>
       <c r="B475" t="n">
-        <v>149.2789001464844</v>
+        <v>149.2788848876953</v>
       </c>
       <c r="C475" t="n">
         <v>149.6454925537109</v>
@@ -11381,7 +11381,7 @@
         <v>44515</v>
       </c>
       <c r="B476" t="n">
-        <v>149.0220336914062</v>
+        <v>149.0220184326172</v>
       </c>
       <c r="C476" t="n">
         <v>149.3880004882812</v>
@@ -11496,7 +11496,7 @@
         <v>44522</v>
       </c>
       <c r="B481" t="n">
-        <v>146.7182006835938</v>
+        <v>146.7181854248047</v>
       </c>
       <c r="C481" t="n">
         <v>147.0785064697266</v>
@@ -11542,7 +11542,7 @@
         <v>44524</v>
       </c>
       <c r="B483" t="n">
-        <v>146.3580780029297</v>
+        <v>146.3580627441406</v>
       </c>
       <c r="C483" t="n">
         <v>146.7174987792969</v>
@@ -11588,7 +11588,7 @@
         <v>44529</v>
       </c>
       <c r="B485" t="n">
-        <v>145.7560577392578</v>
+        <v>145.7560424804688</v>
       </c>
       <c r="C485" t="n">
         <v>146.1139984130859</v>
@@ -11634,7 +11634,7 @@
         <v>44531</v>
       </c>
       <c r="B487" t="n">
-        <v>141.2710723876953</v>
+        <v>141.2710571289062</v>
       </c>
       <c r="C487" t="n">
         <v>141.6179962158203</v>
@@ -11726,7 +11726,7 @@
         <v>44537</v>
       </c>
       <c r="B491" t="n">
-        <v>147.673828125</v>
+        <v>147.6738433837891</v>
       </c>
       <c r="C491" t="n">
         <v>148.0364990234375</v>
@@ -11749,7 +11749,7 @@
         <v>44538</v>
       </c>
       <c r="B492" t="n">
-        <v>148.3561553955078</v>
+        <v>148.3561706542969</v>
       </c>
       <c r="C492" t="n">
         <v>148.7205047607422</v>
@@ -11772,7 +11772,7 @@
         <v>44539</v>
       </c>
       <c r="B493" t="n">
-        <v>147.7431640625</v>
+        <v>147.7431793212891</v>
       </c>
       <c r="C493" t="n">
         <v>148.1060028076172</v>
@@ -11818,7 +11818,7 @@
         <v>44543</v>
       </c>
       <c r="B495" t="n">
-        <v>146.3451080322266</v>
+        <v>146.3450927734375</v>
       </c>
       <c r="C495" t="n">
         <v>146.7044982910156</v>
@@ -12186,7 +12186,7 @@
         <v>44566</v>
       </c>
       <c r="B511" t="n">
-        <v>137.3162841796875</v>
+        <v>137.3162689208984</v>
       </c>
       <c r="C511" t="n">
         <v>137.6535034179688</v>
@@ -12209,7 +12209,7 @@
         <v>44567</v>
       </c>
       <c r="B512" t="n">
-        <v>137.2140350341797</v>
+        <v>137.2140197753906</v>
       </c>
       <c r="C512" t="n">
         <v>137.5509948730469</v>
@@ -12278,7 +12278,7 @@
         <v>44572</v>
       </c>
       <c r="B515" t="n">
-        <v>139.6744842529297</v>
+        <v>139.6744995117188</v>
       </c>
       <c r="C515" t="n">
         <v>140.0175018310547</v>
@@ -12324,7 +12324,7 @@
         <v>44574</v>
       </c>
       <c r="B517" t="n">
-        <v>138.7901611328125</v>
+        <v>138.7901458740234</v>
       </c>
       <c r="C517" t="n">
         <v>139.1309967041016</v>
@@ -12347,7 +12347,7 @@
         <v>44575</v>
       </c>
       <c r="B518" t="n">
-        <v>139.4440460205078</v>
+        <v>139.4440612792969</v>
       </c>
       <c r="C518" t="n">
         <v>139.7864990234375</v>
@@ -12370,7 +12370,7 @@
         <v>44579</v>
       </c>
       <c r="B519" t="n">
-        <v>135.9566040039062</v>
+        <v>135.9566192626953</v>
       </c>
       <c r="C519" t="n">
         <v>136.2904968261719</v>
@@ -12462,7 +12462,7 @@
         <v>44585</v>
       </c>
       <c r="B523" t="n">
-        <v>130.0525970458984</v>
+        <v>130.0526123046875</v>
       </c>
       <c r="C523" t="n">
         <v>130.3719940185547</v>
@@ -12508,7 +12508,7 @@
         <v>44587</v>
       </c>
       <c r="B525" t="n">
-        <v>128.9234008789062</v>
+        <v>128.9233856201172</v>
       </c>
       <c r="C525" t="n">
         <v>129.2400054931641</v>
@@ -12600,7 +12600,7 @@
         <v>44593</v>
       </c>
       <c r="B529" t="n">
-        <v>137.5407104492188</v>
+        <v>137.5407257080078</v>
       </c>
       <c r="C529" t="n">
         <v>137.8784942626953</v>
@@ -12623,7 +12623,7 @@
         <v>44594</v>
       </c>
       <c r="B530" t="n">
-        <v>147.673828125</v>
+        <v>147.6738433837891</v>
       </c>
       <c r="C530" t="n">
         <v>148.0364990234375</v>
@@ -12692,7 +12692,7 @@
         <v>44599</v>
       </c>
       <c r="B533" t="n">
-        <v>138.5976257324219</v>
+        <v>138.5976409912109</v>
       </c>
       <c r="C533" t="n">
         <v>138.9380035400391</v>
@@ -12715,7 +12715,7 @@
         <v>44600</v>
       </c>
       <c r="B534" t="n">
-        <v>138.8719635009766</v>
+        <v>138.8719482421875</v>
       </c>
       <c r="C534" t="n">
         <v>139.2129974365234</v>
@@ -12761,7 +12761,7 @@
         <v>44602</v>
       </c>
       <c r="B536" t="n">
-        <v>138.262939453125</v>
+        <v>138.2629547119141</v>
       </c>
       <c r="C536" t="n">
         <v>138.6024932861328</v>
@@ -12830,7 +12830,7 @@
         <v>44607</v>
       </c>
       <c r="B539" t="n">
-        <v>136.0912780761719</v>
+        <v>136.0912933349609</v>
       </c>
       <c r="C539" t="n">
         <v>136.4255065917969</v>
@@ -12853,7 +12853,7 @@
         <v>44608</v>
       </c>
       <c r="B540" t="n">
-        <v>137.1506805419922</v>
+        <v>137.1506958007812</v>
       </c>
       <c r="C540" t="n">
         <v>137.4875030517578</v>
@@ -12922,7 +12922,7 @@
         <v>44614</v>
       </c>
       <c r="B543" t="n">
-        <v>129.0854949951172</v>
+        <v>129.0854797363281</v>
       </c>
       <c r="C543" t="n">
         <v>129.4024963378906</v>
@@ -12945,7 +12945,7 @@
         <v>44615</v>
       </c>
       <c r="B544" t="n">
-        <v>127.2724380493164</v>
+        <v>127.2724456787109</v>
       </c>
       <c r="C544" t="n">
         <v>127.5849990844727</v>
@@ -12991,7 +12991,7 @@
         <v>44617</v>
       </c>
       <c r="B546" t="n">
-        <v>134.18994140625</v>
+        <v>134.1899566650391</v>
       </c>
       <c r="C546" t="n">
         <v>134.5195007324219</v>
@@ -13014,7 +13014,7 @@
         <v>44620</v>
       </c>
       <c r="B547" t="n">
-        <v>134.5605621337891</v>
+        <v>134.560546875</v>
       </c>
       <c r="C547" t="n">
         <v>134.8910064697266</v>
@@ -13060,7 +13060,7 @@
         <v>44622</v>
       </c>
       <c r="B549" t="n">
-        <v>134.42138671875</v>
+        <v>134.4213714599609</v>
       </c>
       <c r="C549" t="n">
         <v>134.7514953613281</v>
@@ -13129,7 +13129,7 @@
         <v>44627</v>
       </c>
       <c r="B552" t="n">
-        <v>126.1546859741211</v>
+        <v>126.1546936035156</v>
       </c>
       <c r="C552" t="n">
         <v>126.4645004272461</v>
@@ -13244,7 +13244,7 @@
         <v>44634</v>
       </c>
       <c r="B557" t="n">
-        <v>126.4305114746094</v>
+        <v>126.4305038452148</v>
       </c>
       <c r="C557" t="n">
         <v>126.7409973144531</v>
@@ -13313,7 +13313,7 @@
         <v>44637</v>
       </c>
       <c r="B560" t="n">
-        <v>134.270751953125</v>
+        <v>134.2707366943359</v>
       </c>
       <c r="C560" t="n">
         <v>134.6004943847656</v>
@@ -13336,7 +13336,7 @@
         <v>44638</v>
       </c>
       <c r="B561" t="n">
-        <v>136.4663543701172</v>
+        <v>136.4663696289062</v>
       </c>
       <c r="C561" t="n">
         <v>136.8014984130859</v>
@@ -13359,7 +13359,7 @@
         <v>44641</v>
       </c>
       <c r="B562" t="n">
-        <v>136.1441497802734</v>
+        <v>136.1441650390625</v>
       </c>
       <c r="C562" t="n">
         <v>136.4785003662109</v>
@@ -13405,7 +13405,7 @@
         <v>44643</v>
       </c>
       <c r="B564" t="n">
-        <v>138.1641998291016</v>
+        <v>138.1641845703125</v>
       </c>
       <c r="C564" t="n">
         <v>138.5034942626953</v>
@@ -13612,7 +13612,7 @@
         <v>44656</v>
       </c>
       <c r="B573" t="n">
-        <v>140.7174224853516</v>
+        <v>140.7174377441406</v>
       </c>
       <c r="C573" t="n">
         <v>141.0630035400391</v>
@@ -13658,7 +13658,7 @@
         <v>44658</v>
       </c>
       <c r="B575" t="n">
-        <v>136.1306762695312</v>
+        <v>136.1306915283203</v>
       </c>
       <c r="C575" t="n">
         <v>136.4649963378906</v>
@@ -13727,7 +13727,7 @@
         <v>44663</v>
       </c>
       <c r="B578" t="n">
-        <v>128.0599975585938</v>
+        <v>128.0600128173828</v>
       </c>
       <c r="C578" t="n">
         <v>128.3744964599609</v>
@@ -13750,7 +13750,7 @@
         <v>44664</v>
       </c>
       <c r="B579" t="n">
-        <v>129.9668273925781</v>
+        <v>129.9668121337891</v>
       </c>
       <c r="C579" t="n">
         <v>130.2859954833984</v>
@@ -13865,7 +13865,7 @@
         <v>44672</v>
       </c>
       <c r="B584" t="n">
-        <v>124.6314239501953</v>
+        <v>124.6314315795898</v>
       </c>
       <c r="C584" t="n">
         <v>124.9375</v>
@@ -13888,7 +13888,7 @@
         <v>44673</v>
       </c>
       <c r="B585" t="n">
-        <v>119.3209609985352</v>
+        <v>119.3209686279297</v>
       </c>
       <c r="C585" t="n">
         <v>119.6139984130859</v>
@@ -13911,7 +13911,7 @@
         <v>44676</v>
       </c>
       <c r="B586" t="n">
-        <v>122.9480667114258</v>
+        <v>122.9480590820312</v>
       </c>
       <c r="C586" t="n">
         <v>123.25</v>
@@ -13934,7 +13934,7 @@
         <v>44677</v>
       </c>
       <c r="B587" t="n">
-        <v>119.2132263183594</v>
+        <v>119.2132339477539</v>
       </c>
       <c r="C587" t="n">
         <v>119.5059967041016</v>
@@ -14095,7 +14095,7 @@
         <v>44686</v>
       </c>
       <c r="B594" t="n">
-        <v>116.4604949951172</v>
+        <v>116.4604873657227</v>
       </c>
       <c r="C594" t="n">
         <v>116.7464981079102</v>
@@ -14325,7 +14325,7 @@
         <v>44700</v>
       </c>
       <c r="B604" t="n">
-        <v>110.4741973876953</v>
+        <v>110.4741897583008</v>
       </c>
       <c r="C604" t="n">
         <v>110.7454986572266</v>
@@ -14509,7 +14509,7 @@
         <v>44713</v>
       </c>
       <c r="B612" t="n">
-        <v>113.8573837280273</v>
+        <v>113.8573913574219</v>
       </c>
       <c r="C612" t="n">
         <v>114.1370010375977</v>
@@ -14555,7 +14555,7 @@
         <v>44715</v>
       </c>
       <c r="B614" t="n">
-        <v>114.2833480834961</v>
+        <v>114.2833404541016</v>
       </c>
       <c r="C614" t="n">
         <v>114.5640029907227</v>
@@ -14670,7 +14670,7 @@
         <v>44722</v>
       </c>
       <c r="B619" t="n">
-        <v>111.1545181274414</v>
+        <v>111.1545257568359</v>
       </c>
       <c r="C619" t="n">
         <v>111.4274978637695</v>
@@ -14739,7 +14739,7 @@
         <v>44727</v>
       </c>
       <c r="B622" t="n">
-        <v>110.1200714111328</v>
+        <v>110.1200637817383</v>
       </c>
       <c r="C622" t="n">
         <v>110.3905029296875</v>
@@ -14785,7 +14785,7 @@
         <v>44729</v>
       </c>
       <c r="B624" t="n">
-        <v>107.6012573242188</v>
+        <v>107.6012496948242</v>
       </c>
       <c r="C624" t="n">
         <v>107.8655014038086</v>
@@ -14808,7 +14808,7 @@
         <v>44733</v>
       </c>
       <c r="B625" t="n">
-        <v>111.7405853271484</v>
+        <v>111.7405776977539</v>
       </c>
       <c r="C625" t="n">
         <v>112.0149993896484</v>
@@ -14877,7 +14877,7 @@
         <v>44736</v>
       </c>
       <c r="B628" t="n">
-        <v>118.2476119995117</v>
+        <v>118.2476043701172</v>
       </c>
       <c r="C628" t="n">
         <v>118.5380020141602</v>
@@ -14969,7 +14969,7 @@
         <v>44742</v>
       </c>
       <c r="B632" t="n">
-        <v>109.1045532226562</v>
+        <v>109.1045608520508</v>
       </c>
       <c r="C632" t="n">
         <v>109.3724975585938</v>
@@ -15061,7 +15061,7 @@
         <v>44749</v>
       </c>
       <c r="B636" t="n">
-        <v>119.0137176513672</v>
+        <v>119.0137252807617</v>
       </c>
       <c r="C636" t="n">
         <v>119.3059997558594</v>
@@ -15084,7 +15084,7 @@
         <v>44750</v>
       </c>
       <c r="B637" t="n">
-        <v>119.8741149902344</v>
+        <v>119.8741073608398</v>
       </c>
       <c r="C637" t="n">
         <v>120.1685028076172</v>
@@ -15130,7 +15130,7 @@
         <v>44754</v>
       </c>
       <c r="B639" t="n">
-        <v>114.5681381225586</v>
+        <v>114.5681457519531</v>
       </c>
       <c r="C639" t="n">
         <v>114.8495025634766</v>
@@ -15199,7 +15199,7 @@
         <v>44757</v>
       </c>
       <c r="B642" t="n">
-        <v>112.4907379150391</v>
+        <v>112.4907455444336</v>
       </c>
       <c r="C642" t="n">
         <v>112.7669982910156</v>
@@ -15245,7 +15245,7 @@
         <v>44761</v>
       </c>
       <c r="B644" t="n">
-        <v>114.3392028808594</v>
+        <v>114.3392105102539</v>
       </c>
       <c r="C644" t="n">
         <v>114.620002746582</v>
@@ -15268,7 +15268,7 @@
         <v>44762</v>
       </c>
       <c r="B645" t="n">
-        <v>114.4189987182617</v>
+        <v>114.4190063476562</v>
       </c>
       <c r="C645" t="n">
         <v>114.6999969482422</v>
@@ -15291,7 +15291,7 @@
         <v>44763</v>
       </c>
       <c r="B646" t="n">
-        <v>114.7581787109375</v>
+        <v>114.758171081543</v>
       </c>
       <c r="C646" t="n">
         <v>115.0400009155273</v>
@@ -15337,7 +15337,7 @@
         <v>44767</v>
       </c>
       <c r="B648" t="n">
-        <v>107.9449005126953</v>
+        <v>107.9449081420898</v>
       </c>
       <c r="C648" t="n">
         <v>108.2099990844727</v>
@@ -15475,7 +15475,7 @@
         <v>44775</v>
       </c>
       <c r="B654" t="n">
-        <v>115.6160736083984</v>
+        <v>115.6160659790039</v>
       </c>
       <c r="C654" t="n">
         <v>115.9000015258789</v>
@@ -15521,7 +15521,7 @@
         <v>44777</v>
       </c>
       <c r="B656" t="n">
-        <v>118.5787887573242</v>
+        <v>118.5787963867188</v>
       </c>
       <c r="C656" t="n">
         <v>118.870002746582</v>
@@ -15751,7 +15751,7 @@
         <v>44791</v>
       </c>
       <c r="B666" t="n">
-        <v>120.5639190673828</v>
+        <v>120.5639114379883</v>
       </c>
       <c r="C666" t="n">
         <v>120.8600006103516</v>
@@ -15774,7 +15774,7 @@
         <v>44792</v>
       </c>
       <c r="B667" t="n">
-        <v>117.8306350708008</v>
+        <v>117.8306274414062</v>
       </c>
       <c r="C667" t="n">
         <v>118.120002746582</v>
@@ -15820,7 +15820,7 @@
         <v>44796</v>
       </c>
       <c r="B669" t="n">
-        <v>114.4888305664062</v>
+        <v>114.4888381958008</v>
       </c>
       <c r="C669" t="n">
         <v>114.7699966430664</v>
@@ -15843,7 +15843,7 @@
         <v>44797</v>
       </c>
       <c r="B670" t="n">
-        <v>114.4189987182617</v>
+        <v>114.4190063476562</v>
       </c>
       <c r="C670" t="n">
         <v>114.6999969482422</v>
@@ -15889,7 +15889,7 @@
         <v>44799</v>
       </c>
       <c r="B672" t="n">
-        <v>111.0273361206055</v>
+        <v>111.02734375</v>
       </c>
       <c r="C672" t="n">
         <v>111.3000030517578</v>
@@ -15958,7 +15958,7 @@
         <v>44804</v>
       </c>
       <c r="B675" t="n">
-        <v>108.8825988769531</v>
+        <v>108.8826065063477</v>
       </c>
       <c r="C675" t="n">
         <v>109.1500015258789</v>
@@ -15981,7 +15981,7 @@
         <v>44805</v>
       </c>
       <c r="B676" t="n">
-        <v>110.279182434082</v>
+        <v>110.2791748046875</v>
       </c>
       <c r="C676" t="n">
         <v>110.5500030517578</v>
@@ -16004,7 +16004,7 @@
         <v>44806</v>
       </c>
       <c r="B677" t="n">
-        <v>108.4137496948242</v>
+        <v>108.4137573242188</v>
       </c>
       <c r="C677" t="n">
         <v>108.6800003051758</v>
@@ -16073,7 +16073,7 @@
         <v>44812</v>
       </c>
       <c r="B680" t="n">
-        <v>109.1519393920898</v>
+        <v>109.1519470214844</v>
       </c>
       <c r="C680" t="n">
         <v>109.4199981689453</v>
@@ -16096,7 +16096,7 @@
         <v>44813</v>
       </c>
       <c r="B681" t="n">
-        <v>111.5061645507812</v>
+        <v>111.5061569213867</v>
       </c>
       <c r="C681" t="n">
         <v>111.7799987792969</v>
@@ -16142,7 +16142,7 @@
         <v>44817</v>
       </c>
       <c r="B683" t="n">
-        <v>105.052001953125</v>
+        <v>105.0520095825195</v>
       </c>
       <c r="C683" t="n">
         <v>105.3099975585938</v>
@@ -16211,7 +16211,7 @@
         <v>44820</v>
       </c>
       <c r="B686" t="n">
-        <v>103.3761291503906</v>
+        <v>103.3761215209961</v>
       </c>
       <c r="C686" t="n">
         <v>103.629997253418</v>
@@ -16234,7 +16234,7 @@
         <v>44823</v>
       </c>
       <c r="B687" t="n">
-        <v>103.595588684082</v>
+        <v>103.5955810546875</v>
       </c>
       <c r="C687" t="n">
         <v>103.8499984741211</v>
@@ -16326,7 +16326,7 @@
         <v>44827</v>
       </c>
       <c r="B691" t="n">
-        <v>98.92704772949219</v>
+        <v>98.92705535888672</v>
       </c>
       <c r="C691" t="n">
         <v>99.16999816894531</v>
@@ -16464,7 +16464,7 @@
         <v>44837</v>
       </c>
       <c r="B697" t="n">
-        <v>99.05673980712891</v>
+        <v>99.05673217773438</v>
       </c>
       <c r="C697" t="n">
         <v>99.30000305175781</v>
@@ -16487,7 +16487,7 @@
         <v>44838</v>
       </c>
       <c r="B698" t="n">
-        <v>102.1591262817383</v>
+        <v>102.1591186523438</v>
       </c>
       <c r="C698" t="n">
         <v>102.4100036621094</v>
@@ -16740,7 +16740,7 @@
         <v>44853</v>
       </c>
       <c r="B709" t="n">
-        <v>100.044303894043</v>
+        <v>100.0443115234375</v>
       </c>
       <c r="C709" t="n">
         <v>100.2900009155273</v>
@@ -16763,7 +16763,7 @@
         <v>44854</v>
       </c>
       <c r="B710" t="n">
-        <v>100.2837219238281</v>
+        <v>100.2837142944336</v>
       </c>
       <c r="C710" t="n">
         <v>100.5299987792969</v>
@@ -16924,7 +16924,7 @@
         <v>44865</v>
       </c>
       <c r="B717" t="n">
-        <v>94.4281005859375</v>
+        <v>94.42810821533203</v>
       </c>
       <c r="C717" t="n">
         <v>94.66000366210938</v>
@@ -16947,7 +16947,7 @@
         <v>44866</v>
       </c>
       <c r="B718" t="n">
-        <v>90.27828979492188</v>
+        <v>90.27829742431641</v>
       </c>
       <c r="C718" t="n">
         <v>90.5</v>
@@ -16993,7 +16993,7 @@
         <v>44868</v>
       </c>
       <c r="B720" t="n">
-        <v>83.28546142578125</v>
+        <v>83.28546905517578</v>
       </c>
       <c r="C720" t="n">
         <v>83.48999786376953</v>
@@ -17016,7 +17016,7 @@
         <v>44869</v>
       </c>
       <c r="B721" t="n">
-        <v>86.48759460449219</v>
+        <v>86.48760223388672</v>
       </c>
       <c r="C721" t="n">
         <v>86.69999694824219</v>
@@ -17039,7 +17039,7 @@
         <v>44872</v>
       </c>
       <c r="B722" t="n">
-        <v>88.43283081054688</v>
+        <v>88.43282318115234</v>
       </c>
       <c r="C722" t="n">
         <v>88.65000152587891</v>
@@ -17223,7 +17223,7 @@
         <v>44882</v>
       </c>
       <c r="B730" t="n">
-        <v>98.25869750976562</v>
+        <v>98.25868988037109</v>
       </c>
       <c r="C730" t="n">
         <v>98.5</v>
@@ -17315,7 +17315,7 @@
         <v>44888</v>
       </c>
       <c r="B734" t="n">
-        <v>98.57790374755859</v>
+        <v>98.57791137695312</v>
       </c>
       <c r="C734" t="n">
         <v>98.81999969482422</v>
@@ -17407,7 +17407,7 @@
         <v>44895</v>
       </c>
       <c r="B738" t="n">
-        <v>101.2014694213867</v>
+        <v>101.2014617919922</v>
       </c>
       <c r="C738" t="n">
         <v>101.4499969482422</v>
@@ -17453,7 +17453,7 @@
         <v>44897</v>
       </c>
       <c r="B740" t="n">
-        <v>100.5829849243164</v>
+        <v>100.5829925537109</v>
       </c>
       <c r="C740" t="n">
         <v>100.8300018310547</v>
@@ -17476,7 +17476,7 @@
         <v>44900</v>
       </c>
       <c r="B741" t="n">
-        <v>99.62534332275391</v>
+        <v>99.62533569335938</v>
       </c>
       <c r="C741" t="n">
         <v>99.87000274658203</v>
@@ -17545,7 +17545,7 @@
         <v>44903</v>
       </c>
       <c r="B744" t="n">
-        <v>93.71984100341797</v>
+        <v>93.71983337402344</v>
       </c>
       <c r="C744" t="n">
         <v>93.94999694824219</v>
@@ -17591,7 +17591,7 @@
         <v>44907</v>
       </c>
       <c r="B746" t="n">
-        <v>93.33079528808594</v>
+        <v>93.33078765869141</v>
       </c>
       <c r="C746" t="n">
         <v>93.55999755859375</v>
@@ -17660,7 +17660,7 @@
         <v>44910</v>
       </c>
       <c r="B749" t="n">
-        <v>90.97657775878906</v>
+        <v>90.97657012939453</v>
       </c>
       <c r="C749" t="n">
         <v>91.19999694824219</v>
@@ -17683,7 +17683,7 @@
         <v>44911</v>
       </c>
       <c r="B750" t="n">
-        <v>90.63740539550781</v>
+        <v>90.63741302490234</v>
       </c>
       <c r="C750" t="n">
         <v>90.86000061035156</v>
@@ -17752,7 +17752,7 @@
         <v>44916</v>
       </c>
       <c r="B753" t="n">
-        <v>90.02890014648438</v>
+        <v>90.02890777587891</v>
       </c>
       <c r="C753" t="n">
         <v>90.25</v>
@@ -17913,7 +17913,7 @@
         <v>44929</v>
       </c>
       <c r="B760" t="n">
-        <v>89.48024749755859</v>
+        <v>89.48025512695312</v>
       </c>
       <c r="C760" t="n">
         <v>89.69999694824219</v>
@@ -17936,7 +17936,7 @@
         <v>44930</v>
       </c>
       <c r="B761" t="n">
-        <v>88.49268341064453</v>
+        <v>88.49267578125</v>
       </c>
       <c r="C761" t="n">
         <v>88.70999908447266</v>
@@ -18005,7 +18005,7 @@
         <v>44935</v>
       </c>
       <c r="B764" t="n">
-        <v>88.58245849609375</v>
+        <v>88.58246612548828</v>
       </c>
       <c r="C764" t="n">
         <v>88.80000305175781</v>
@@ -18051,7 +18051,7 @@
         <v>44937</v>
       </c>
       <c r="B766" t="n">
-        <v>92.03398895263672</v>
+        <v>92.03398132324219</v>
       </c>
       <c r="C766" t="n">
         <v>92.26000213623047</v>
@@ -18097,7 +18097,7 @@
         <v>44939</v>
       </c>
       <c r="B768" t="n">
-        <v>92.57266235351562</v>
+        <v>92.57265472412109</v>
       </c>
       <c r="C768" t="n">
         <v>92.80000305175781</v>
@@ -18166,7 +18166,7 @@
         <v>44945</v>
       </c>
       <c r="B771" t="n">
-        <v>93.67994689941406</v>
+        <v>93.67993927001953</v>
       </c>
       <c r="C771" t="n">
         <v>93.91000366210938</v>
@@ -18235,7 +18235,7 @@
         <v>44950</v>
       </c>
       <c r="B774" t="n">
-        <v>98.96694946289062</v>
+        <v>98.96695709228516</v>
       </c>
       <c r="C774" t="n">
         <v>99.20999908447266</v>
@@ -18281,7 +18281,7 @@
         <v>44952</v>
       </c>
       <c r="B776" t="n">
-        <v>98.91708374023438</v>
+        <v>98.91707611083984</v>
       </c>
       <c r="C776" t="n">
         <v>99.16000366210938</v>
@@ -18350,7 +18350,7 @@
         <v>44957</v>
       </c>
       <c r="B779" t="n">
-        <v>99.62534332275391</v>
+        <v>99.62533569335938</v>
       </c>
       <c r="C779" t="n">
         <v>99.87000274658203</v>
@@ -18373,7 +18373,7 @@
         <v>44958</v>
       </c>
       <c r="B780" t="n">
-        <v>101.1815185546875</v>
+        <v>101.181510925293</v>
       </c>
       <c r="C780" t="n">
         <v>101.4300003051758</v>
@@ -18419,7 +18419,7 @@
         <v>44960</v>
       </c>
       <c r="B782" t="n">
-        <v>104.9622344970703</v>
+        <v>104.9622268676758</v>
       </c>
       <c r="C782" t="n">
         <v>105.2200012207031</v>
@@ -18465,7 +18465,7 @@
         <v>44964</v>
       </c>
       <c r="B784" t="n">
-        <v>107.7753295898438</v>
+        <v>107.7753219604492</v>
       </c>
       <c r="C784" t="n">
         <v>108.0400009155273</v>
@@ -18718,7 +18718,7 @@
         <v>44980</v>
       </c>
       <c r="B795" t="n">
-        <v>90.84689331054688</v>
+        <v>90.84690093994141</v>
       </c>
       <c r="C795" t="n">
         <v>91.06999969482422</v>
@@ -18741,7 +18741,7 @@
         <v>44981</v>
       </c>
       <c r="B796" t="n">
-        <v>89.131103515625</v>
+        <v>89.13111114501953</v>
       </c>
       <c r="C796" t="n">
         <v>89.34999847412109</v>
@@ -18787,7 +18787,7 @@
         <v>44985</v>
       </c>
       <c r="B798" t="n">
-        <v>90.07878875732422</v>
+        <v>90.07878112792969</v>
       </c>
       <c r="C798" t="n">
         <v>90.30000305175781</v>
@@ -19017,7 +19017,7 @@
         <v>44999</v>
       </c>
       <c r="B808" t="n">
-        <v>94.01910400390625</v>
+        <v>94.01911163330078</v>
       </c>
       <c r="C808" t="n">
         <v>94.25</v>
@@ -19040,7 +19040,7 @@
         <v>45000</v>
       </c>
       <c r="B809" t="n">
-        <v>96.3134765625</v>
+        <v>96.31346893310547</v>
       </c>
       <c r="C809" t="n">
         <v>96.55000305175781</v>
@@ -19224,7 +19224,7 @@
         <v>45012</v>
       </c>
       <c r="B817" t="n">
-        <v>102.8075256347656</v>
+        <v>102.8075180053711</v>
       </c>
       <c r="C817" t="n">
         <v>103.0599975585938</v>
@@ -19339,7 +19339,7 @@
         <v>45019</v>
       </c>
       <c r="B822" t="n">
-        <v>104.6529922485352</v>
+        <v>104.6529998779297</v>
       </c>
       <c r="C822" t="n">
         <v>104.9100036621094</v>
@@ -19385,7 +19385,7 @@
         <v>45021</v>
       </c>
       <c r="B824" t="n">
-        <v>104.6928863525391</v>
+        <v>104.6928939819336</v>
       </c>
       <c r="C824" t="n">
         <v>104.9499969482422</v>
@@ -19477,7 +19477,7 @@
         <v>45028</v>
       </c>
       <c r="B828" t="n">
-        <v>104.9622344970703</v>
+        <v>104.9622268676758</v>
       </c>
       <c r="C828" t="n">
         <v>105.2200012207031</v>
@@ -19500,7 +19500,7 @@
         <v>45029</v>
       </c>
       <c r="B829" t="n">
-        <v>107.9249572753906</v>
+        <v>107.9249649047852</v>
       </c>
       <c r="C829" t="n">
         <v>108.1900024414062</v>
@@ -19523,7 +19523,7 @@
         <v>45030</v>
       </c>
       <c r="B830" t="n">
-        <v>109.1918411254883</v>
+        <v>109.1918487548828</v>
       </c>
       <c r="C830" t="n">
         <v>109.4599990844727</v>
@@ -19546,7 +19546,7 @@
         <v>45033</v>
       </c>
       <c r="B831" t="n">
-        <v>106.1592864990234</v>
+        <v>106.159294128418</v>
       </c>
       <c r="C831" t="n">
         <v>106.4199981689453</v>
@@ -19615,7 +19615,7 @@
         <v>45036</v>
       </c>
       <c r="B834" t="n">
-        <v>105.6405715942383</v>
+        <v>105.6405639648438</v>
       </c>
       <c r="C834" t="n">
         <v>105.9000015258789</v>
@@ -19684,7 +19684,7 @@
         <v>45041</v>
       </c>
       <c r="B837" t="n">
-        <v>104.3537292480469</v>
+        <v>104.3537216186523</v>
       </c>
       <c r="C837" t="n">
         <v>104.6100006103516</v>
@@ -19730,7 +19730,7 @@
         <v>45043</v>
       </c>
       <c r="B839" t="n">
-        <v>108.1045227050781</v>
+        <v>108.1045150756836</v>
       </c>
       <c r="C839" t="n">
         <v>108.370002746582</v>
@@ -19753,7 +19753,7 @@
         <v>45044</v>
       </c>
       <c r="B840" t="n">
-        <v>107.9548873901367</v>
+        <v>107.9548797607422</v>
       </c>
       <c r="C840" t="n">
         <v>108.2200012207031</v>
@@ -19799,7 +19799,7 @@
         <v>45048</v>
       </c>
       <c r="B842" t="n">
-        <v>105.7203750610352</v>
+        <v>105.7203674316406</v>
       </c>
       <c r="C842" t="n">
         <v>105.9800033569336</v>
@@ -19868,7 +19868,7 @@
         <v>45051</v>
       </c>
       <c r="B845" t="n">
-        <v>105.9547958374023</v>
+        <v>105.9547882080078</v>
       </c>
       <c r="C845" t="n">
         <v>106.2149963378906</v>
@@ -20075,7 +20075,7 @@
         <v>45064</v>
       </c>
       <c r="B854" t="n">
-        <v>123.2173919677734</v>
+        <v>123.217399597168</v>
       </c>
       <c r="C854" t="n">
         <v>123.5199966430664</v>
@@ -20098,7 +20098,7 @@
         <v>45065</v>
       </c>
       <c r="B855" t="n">
-        <v>122.9480667114258</v>
+        <v>122.9480590820312</v>
       </c>
       <c r="C855" t="n">
         <v>123.25</v>
@@ -20167,7 +20167,7 @@
         <v>45070</v>
       </c>
       <c r="B858" t="n">
-        <v>121.3420104980469</v>
+        <v>121.3420028686523</v>
       </c>
       <c r="C858" t="n">
         <v>121.6399993896484</v>
@@ -20282,7 +20282,7 @@
         <v>45078</v>
       </c>
       <c r="B863" t="n">
-        <v>124.0653228759766</v>
+        <v>124.065315246582</v>
       </c>
       <c r="C863" t="n">
         <v>124.370002746582</v>
@@ -20305,7 +20305,7 @@
         <v>45079</v>
       </c>
       <c r="B864" t="n">
-        <v>124.9232177734375</v>
+        <v>124.923210144043</v>
       </c>
       <c r="C864" t="n">
         <v>125.2300033569336</v>
@@ -20466,7 +20466,7 @@
         <v>45090</v>
       </c>
       <c r="B871" t="n">
-        <v>124.1251754760742</v>
+        <v>124.1251678466797</v>
       </c>
       <c r="C871" t="n">
         <v>124.4300003051758</v>
@@ -20489,7 +20489,7 @@
         <v>45091</v>
       </c>
       <c r="B872" t="n">
-        <v>124.0752868652344</v>
+        <v>124.0752944946289</v>
       </c>
       <c r="C872" t="n">
         <v>124.379997253418</v>
@@ -20512,7 +20512,7 @@
         <v>45092</v>
       </c>
       <c r="B873" t="n">
-        <v>125.4818344116211</v>
+        <v>125.4818420410156</v>
       </c>
       <c r="C873" t="n">
         <v>125.7900009155273</v>
@@ -20558,7 +20558,7 @@
         <v>45097</v>
       </c>
       <c r="B875" t="n">
-        <v>123.5465850830078</v>
+        <v>123.5465927124023</v>
       </c>
       <c r="C875" t="n">
         <v>123.8499984741211</v>
@@ -20604,7 +20604,7 @@
         <v>45099</v>
       </c>
       <c r="B877" t="n">
-        <v>123.5665435791016</v>
+        <v>123.5665512084961</v>
       </c>
       <c r="C877" t="n">
         <v>123.870002746582</v>
@@ -20673,7 +20673,7 @@
         <v>45104</v>
       </c>
       <c r="B880" t="n">
-        <v>118.7184448242188</v>
+        <v>118.7184524536133</v>
       </c>
       <c r="C880" t="n">
         <v>119.0100021362305</v>
@@ -20719,7 +20719,7 @@
         <v>45106</v>
       </c>
       <c r="B882" t="n">
-        <v>119.7159957885742</v>
+        <v>119.7160034179688</v>
       </c>
       <c r="C882" t="n">
         <v>120.0100021362305</v>
@@ -20903,7 +20903,7 @@
         <v>45119</v>
       </c>
       <c r="B890" t="n">
-        <v>119.3269500732422</v>
+        <v>119.3269577026367</v>
       </c>
       <c r="C890" t="n">
         <v>119.620002746582</v>
@@ -20949,7 +20949,7 @@
         <v>45121</v>
       </c>
       <c r="B892" t="n">
-        <v>125.3920593261719</v>
+        <v>125.3920516967773</v>
       </c>
       <c r="C892" t="n">
         <v>125.6999969482422</v>
@@ -20972,7 +20972,7 @@
         <v>45124</v>
       </c>
       <c r="B893" t="n">
-        <v>124.7536239624023</v>
+        <v>124.7536315917969</v>
       </c>
       <c r="C893" t="n">
         <v>125.0599975585938</v>
@@ -20995,7 +20995,7 @@
         <v>45125</v>
       </c>
       <c r="B894" t="n">
-        <v>123.7760314941406</v>
+        <v>123.7760238647461</v>
       </c>
       <c r="C894" t="n">
         <v>124.0800018310547</v>
@@ -21018,7 +21018,7 @@
         <v>45126</v>
       </c>
       <c r="B895" t="n">
-        <v>122.4792175292969</v>
+        <v>122.4792098999023</v>
       </c>
       <c r="C895" t="n">
         <v>122.7799987792969</v>
@@ -21041,7 +21041,7 @@
         <v>45127</v>
       </c>
       <c r="B896" t="n">
-        <v>119.237174987793</v>
+        <v>119.2371673583984</v>
       </c>
       <c r="C896" t="n">
         <v>119.5299987792969</v>
@@ -21064,7 +21064,7 @@
         <v>45128</v>
       </c>
       <c r="B897" t="n">
-        <v>120.015266418457</v>
+        <v>120.0152587890625</v>
       </c>
       <c r="C897" t="n">
         <v>120.3099975585938</v>
@@ -21087,7 +21087,7 @@
         <v>45131</v>
       </c>
       <c r="B898" t="n">
-        <v>121.581413269043</v>
+        <v>121.5814208984375</v>
       </c>
       <c r="C898" t="n">
         <v>121.879997253418</v>
@@ -21156,7 +21156,7 @@
         <v>45134</v>
       </c>
       <c r="B901" t="n">
-        <v>129.5518493652344</v>
+        <v>129.5518341064453</v>
       </c>
       <c r="C901" t="n">
         <v>129.8699951171875</v>
@@ -21248,7 +21248,7 @@
         <v>45140</v>
       </c>
       <c r="B905" t="n">
-        <v>128.3248443603516</v>
+        <v>128.3248596191406</v>
       </c>
       <c r="C905" t="n">
         <v>128.6399993896484</v>
@@ -21294,7 +21294,7 @@
         <v>45142</v>
       </c>
       <c r="B907" t="n">
-        <v>128.22509765625</v>
+        <v>128.2250823974609</v>
       </c>
       <c r="C907" t="n">
         <v>128.5399932861328</v>
@@ -21386,7 +21386,7 @@
         <v>45148</v>
       </c>
       <c r="B911" t="n">
-        <v>129.8910064697266</v>
+        <v>129.8910217285156</v>
       </c>
       <c r="C911" t="n">
         <v>130.2100067138672</v>
@@ -21547,7 +21547,7 @@
         <v>45159</v>
       </c>
       <c r="B918" t="n">
-        <v>128.6141510009766</v>
+        <v>128.6141357421875</v>
       </c>
       <c r="C918" t="n">
         <v>128.9299926757812</v>
@@ -21616,7 +21616,7 @@
         <v>45162</v>
       </c>
       <c r="B921" t="n">
-        <v>130.1004943847656</v>
+        <v>130.1005096435547</v>
       </c>
       <c r="C921" t="n">
         <v>130.4199981689453</v>
@@ -21639,7 +21639,7 @@
         <v>45163</v>
       </c>
       <c r="B922" t="n">
-        <v>130.3698425292969</v>
+        <v>130.3698272705078</v>
       </c>
       <c r="C922" t="n">
         <v>130.6900024414062</v>
@@ -21754,7 +21754,7 @@
         <v>45170</v>
       </c>
       <c r="B927" t="n">
-        <v>136.4648590087891</v>
+        <v>136.4648742675781</v>
       </c>
       <c r="C927" t="n">
         <v>136.8000030517578</v>
@@ -21777,7 +21777,7 @@
         <v>45174</v>
       </c>
       <c r="B928" t="n">
-        <v>136.3750915527344</v>
+        <v>136.3751068115234</v>
       </c>
       <c r="C928" t="n">
         <v>136.7100067138672</v>
@@ -21823,7 +21823,7 @@
         <v>45176</v>
       </c>
       <c r="B930" t="n">
-        <v>135.8663330078125</v>
+        <v>135.8663482666016</v>
       </c>
       <c r="C930" t="n">
         <v>136.1999969482422</v>
@@ -21846,7 +21846,7 @@
         <v>45177</v>
       </c>
       <c r="B931" t="n">
-        <v>136.8638916015625</v>
+        <v>136.8638763427734</v>
       </c>
       <c r="C931" t="n">
         <v>137.1999969482422</v>
@@ -21869,7 +21869,7 @@
         <v>45180</v>
       </c>
       <c r="B932" t="n">
-        <v>137.4025573730469</v>
+        <v>137.4025726318359</v>
       </c>
       <c r="C932" t="n">
         <v>137.7400054931641</v>
@@ -21915,7 +21915,7 @@
         <v>45182</v>
       </c>
       <c r="B934" t="n">
-        <v>137.1631469726562</v>
+        <v>137.1631622314453</v>
       </c>
       <c r="C934" t="n">
         <v>137.5</v>
@@ -22053,7 +22053,7 @@
         <v>45190</v>
       </c>
       <c r="B940" t="n">
-        <v>131.0381927490234</v>
+        <v>131.0382080078125</v>
       </c>
       <c r="C940" t="n">
         <v>131.3600006103516</v>
@@ -22260,7 +22260,7 @@
         <v>45203</v>
       </c>
       <c r="B949" t="n">
-        <v>135.9361724853516</v>
+        <v>135.9361572265625</v>
       </c>
       <c r="C949" t="n">
         <v>136.2700042724609</v>
@@ -22352,7 +22352,7 @@
         <v>45209</v>
       </c>
       <c r="B953" t="n">
-        <v>138.8589935302734</v>
+        <v>138.8589782714844</v>
       </c>
       <c r="C953" t="n">
         <v>139.1999969482422</v>
@@ -22421,7 +22421,7 @@
         <v>45212</v>
       </c>
       <c r="B956" t="n">
-        <v>138.2405090332031</v>
+        <v>138.2404937744141</v>
       </c>
       <c r="C956" t="n">
         <v>138.5800018310547</v>
@@ -22444,7 +22444,7 @@
         <v>45215</v>
       </c>
       <c r="B957" t="n">
-        <v>140.1458435058594</v>
+        <v>140.1458282470703</v>
       </c>
       <c r="C957" t="n">
         <v>140.4900054931641</v>
@@ -22490,7 +22490,7 @@
         <v>45217</v>
       </c>
       <c r="B959" t="n">
-        <v>138.9387969970703</v>
+        <v>138.9387817382812</v>
       </c>
       <c r="C959" t="n">
         <v>139.2799987792969</v>
@@ -22559,7 +22559,7 @@
         <v>45222</v>
       </c>
       <c r="B962" t="n">
-        <v>137.5621795654297</v>
+        <v>137.5621643066406</v>
       </c>
       <c r="C962" t="n">
         <v>137.8999938964844</v>
@@ -22628,7 +22628,7 @@
         <v>45225</v>
       </c>
       <c r="B965" t="n">
-        <v>123.1375961303711</v>
+        <v>123.1376037597656</v>
       </c>
       <c r="C965" t="n">
         <v>123.4400024414062</v>
@@ -22674,7 +22674,7 @@
         <v>45229</v>
       </c>
       <c r="B967" t="n">
-        <v>125.4419326782227</v>
+        <v>125.4419403076172</v>
       </c>
       <c r="C967" t="n">
         <v>125.75</v>
@@ -22743,7 +22743,7 @@
         <v>45232</v>
       </c>
       <c r="B970" t="n">
-        <v>128.2650146484375</v>
+        <v>128.2649993896484</v>
       </c>
       <c r="C970" t="n">
         <v>128.5800018310547</v>
@@ -23042,7 +23042,7 @@
         <v>45251</v>
       </c>
       <c r="B983" t="n">
-        <v>138.2804107666016</v>
+        <v>138.2803955078125</v>
       </c>
       <c r="C983" t="n">
         <v>138.6199951171875</v>
@@ -23065,7 +23065,7 @@
         <v>45252</v>
       </c>
       <c r="B984" t="n">
-        <v>139.6769866943359</v>
+        <v>139.6769714355469</v>
       </c>
       <c r="C984" t="n">
         <v>140.0200042724609</v>
@@ -23088,7 +23088,7 @@
         <v>45254</v>
       </c>
       <c r="B985" t="n">
-        <v>137.8813934326172</v>
+        <v>137.8813781738281</v>
       </c>
       <c r="C985" t="n">
         <v>138.2200012207031</v>
@@ -23134,7 +23134,7 @@
         <v>45258</v>
       </c>
       <c r="B987" t="n">
-        <v>138.2804107666016</v>
+        <v>138.2803955078125</v>
       </c>
       <c r="C987" t="n">
         <v>138.6199951171875</v>
@@ -23318,7 +23318,7 @@
         <v>45268</v>
       </c>
       <c r="B995" t="n">
-        <v>136.3052520751953</v>
+        <v>136.3052673339844</v>
       </c>
       <c r="C995" t="n">
         <v>136.6399993896484</v>
@@ -23755,7 +23755,7 @@
         <v>45299</v>
       </c>
       <c r="B1014" t="n">
-        <v>140.1857299804688</v>
+        <v>140.1857147216797</v>
       </c>
       <c r="C1014" t="n">
         <v>140.5299987792969</v>
@@ -23916,7 +23916,7 @@
         <v>45309</v>
       </c>
       <c r="B1021" t="n">
-        <v>144.6347961425781</v>
+        <v>144.6348114013672</v>
       </c>
       <c r="C1021" t="n">
         <v>144.9900054931641</v>
@@ -23985,7 +23985,7 @@
         <v>45314</v>
       </c>
       <c r="B1024" t="n">
-        <v>148.3157653808594</v>
+        <v>148.3157501220703</v>
       </c>
       <c r="C1024" t="n">
         <v>148.6799926757812</v>
@@ -24192,7 +24192,7 @@
         <v>45327</v>
       </c>
       <c r="B1033" t="n">
-        <v>144.574951171875</v>
+        <v>144.5749359130859</v>
       </c>
       <c r="C1033" t="n">
         <v>144.9299926757812</v>
@@ -24238,7 +24238,7 @@
         <v>45329</v>
       </c>
       <c r="B1035" t="n">
-        <v>146.3206481933594</v>
+        <v>146.3206634521484</v>
       </c>
       <c r="C1035" t="n">
         <v>146.6799926757812</v>
@@ -24261,7 +24261,7 @@
         <v>45330</v>
       </c>
       <c r="B1036" t="n">
-        <v>146.8593292236328</v>
+        <v>146.8593444824219</v>
       </c>
       <c r="C1036" t="n">
         <v>147.2200012207031</v>
@@ -24307,7 +24307,7 @@
         <v>45334</v>
       </c>
       <c r="B1038" t="n">
-        <v>148.3656463623047</v>
+        <v>148.3656311035156</v>
       </c>
       <c r="C1038" t="n">
         <v>148.7299957275391</v>
@@ -24330,7 +24330,7 @@
         <v>45335</v>
       </c>
       <c r="B1039" t="n">
-        <v>146.0114288330078</v>
+        <v>146.0114135742188</v>
       </c>
       <c r="C1039" t="n">
         <v>146.3699951171875</v>
@@ -24353,7 +24353,7 @@
         <v>45336</v>
       </c>
       <c r="B1040" t="n">
-        <v>146.7795257568359</v>
+        <v>146.779541015625</v>
       </c>
       <c r="C1040" t="n">
         <v>147.1399993896484</v>
@@ -24491,7 +24491,7 @@
         <v>45345</v>
       </c>
       <c r="B1046" t="n">
-        <v>144.9340667724609</v>
+        <v>144.9340515136719</v>
       </c>
       <c r="C1046" t="n">
         <v>145.2899932861328</v>
@@ -24514,7 +24514,7 @@
         <v>45348</v>
       </c>
       <c r="B1047" t="n">
-        <v>138.4100799560547</v>
+        <v>138.4100952148438</v>
       </c>
       <c r="C1047" t="n">
         <v>138.75</v>
@@ -24606,7 +24606,7 @@
         <v>45352</v>
       </c>
       <c r="B1051" t="n">
-        <v>137.7417297363281</v>
+        <v>137.7417449951172</v>
       </c>
       <c r="C1051" t="n">
         <v>138.0800018310547</v>
@@ -24652,7 +24652,7 @@
         <v>45356</v>
       </c>
       <c r="B1053" t="n">
-        <v>133.4522552490234</v>
+        <v>133.4522705078125</v>
       </c>
       <c r="C1053" t="n">
         <v>133.7799987792969</v>
@@ -24721,7 +24721,7 @@
         <v>45359</v>
       </c>
       <c r="B1056" t="n">
-        <v>135.9561004638672</v>
+        <v>135.9561157226562</v>
       </c>
       <c r="C1056" t="n">
         <v>136.2899932861328</v>
@@ -24859,7 +24859,7 @@
         <v>45369</v>
       </c>
       <c r="B1062" t="n">
-        <v>148.1162414550781</v>
+        <v>148.1162567138672</v>
       </c>
       <c r="C1062" t="n">
         <v>148.4799957275391</v>
@@ -24882,7 +24882,7 @@
         <v>45370</v>
       </c>
       <c r="B1063" t="n">
-        <v>147.5576171875</v>
+        <v>147.5576324462891</v>
       </c>
       <c r="C1063" t="n">
         <v>147.9199981689453</v>
@@ -24974,7 +24974,7 @@
         <v>45376</v>
       </c>
       <c r="B1067" t="n">
-        <v>150.7797088623047</v>
+        <v>150.7796936035156</v>
       </c>
       <c r="C1067" t="n">
         <v>151.1499938964844</v>
@@ -24997,7 +24997,7 @@
         <v>45377</v>
       </c>
       <c r="B1068" t="n">
-        <v>151.328369140625</v>
+        <v>151.3283538818359</v>
       </c>
       <c r="C1068" t="n">
         <v>151.6999969482422</v>
@@ -25204,7 +25204,7 @@
         <v>45391</v>
       </c>
       <c r="B1077" t="n">
-        <v>157.7525939941406</v>
+        <v>157.7525787353516</v>
       </c>
       <c r="C1077" t="n">
         <v>158.1399993896484</v>
@@ -25296,7 +25296,7 @@
         <v>45397</v>
       </c>
       <c r="B1081" t="n">
-        <v>155.9470367431641</v>
+        <v>155.947021484375</v>
       </c>
       <c r="C1081" t="n">
         <v>156.3300018310547</v>
@@ -25365,7 +25365,7 @@
         <v>45400</v>
       </c>
       <c r="B1084" t="n">
-        <v>157.0742492675781</v>
+        <v>157.0742645263672</v>
       </c>
       <c r="C1084" t="n">
         <v>157.4600067138672</v>
@@ -25526,7 +25526,7 @@
         <v>45411</v>
       </c>
       <c r="B1091" t="n">
-        <v>167.4886779785156</v>
+        <v>167.4886627197266</v>
       </c>
       <c r="C1091" t="n">
         <v>167.8999938964844</v>
@@ -25572,7 +25572,7 @@
         <v>45413</v>
       </c>
       <c r="B1093" t="n">
-        <v>165.1643829345703</v>
+        <v>165.1643981933594</v>
       </c>
       <c r="C1093" t="n">
         <v>165.5700073242188</v>
@@ -25618,7 +25618,7 @@
         <v>45415</v>
       </c>
       <c r="B1095" t="n">
-        <v>168.5760192871094</v>
+        <v>168.5760040283203</v>
       </c>
       <c r="C1095" t="n">
         <v>168.9900054931641</v>
@@ -25710,7 +25710,7 @@
         <v>45421</v>
       </c>
       <c r="B1099" t="n">
-        <v>171.15966796875</v>
+        <v>171.1596527099609</v>
       </c>
       <c r="C1099" t="n">
         <v>171.5800018310547</v>
@@ -25733,7 +25733,7 @@
         <v>45422</v>
       </c>
       <c r="B1100" t="n">
-        <v>169.8728179931641</v>
+        <v>169.872802734375</v>
       </c>
       <c r="C1100" t="n">
         <v>170.2899932861328</v>
@@ -25779,7 +25779,7 @@
         <v>45426</v>
       </c>
       <c r="B1102" t="n">
-        <v>171.5088043212891</v>
+        <v>171.5087890625</v>
       </c>
       <c r="C1102" t="n">
         <v>171.9299926757812</v>
@@ -25871,7 +25871,7 @@
         <v>45432</v>
       </c>
       <c r="B1106" t="n">
-        <v>178.0228118896484</v>
+        <v>178.0228271484375</v>
       </c>
       <c r="C1106" t="n">
         <v>178.4600067138672</v>
@@ -25986,7 +25986,7 @@
         <v>45440</v>
       </c>
       <c r="B1111" t="n">
-        <v>177.5838928222656</v>
+        <v>177.5838775634766</v>
       </c>
       <c r="C1111" t="n">
         <v>178.0200042724609</v>
@@ -26101,7 +26101,7 @@
         <v>45447</v>
       </c>
       <c r="B1116" t="n">
-        <v>174.7009735107422</v>
+        <v>174.7009582519531</v>
       </c>
       <c r="C1116" t="n">
         <v>175.1300048828125</v>
@@ -26124,7 +26124,7 @@
         <v>45448</v>
       </c>
       <c r="B1117" t="n">
-        <v>176.63623046875</v>
+        <v>176.6362152099609</v>
       </c>
       <c r="C1117" t="n">
         <v>177.0700073242188</v>
@@ -26147,7 +26147,7 @@
         <v>45449</v>
       </c>
       <c r="B1118" t="n">
-        <v>177.9130706787109</v>
+        <v>177.9130859375</v>
       </c>
       <c r="C1118" t="n">
         <v>178.3500061035156</v>

</xml_diff>